<commit_message>
Changes are related to frontend status check
</commit_message>
<xml_diff>
--- a/DbScript/Config.xlsx
+++ b/DbScript/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydutt\source\test\TestDataGen\DbScript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Piyali\Tasks\Short_Term_Goal\TestdataGenerationTool\TestDataGen\DbScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D95F0A3-1A61-4ABB-8F0C-72024FDF6FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669DF161-BCF7-416B-BB5C-0258178C32FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>Username</t>
   </si>
   <si>
-    <t>extendhealth\jaydutt</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
@@ -101,6 +98,9 @@
   </si>
   <si>
     <t>MSSQLSERVER</t>
+  </si>
+  <si>
+    <t>extendhealth\piroy</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,34 +481,34 @@
         <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +546,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -568,10 +568,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -585,10 +585,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -602,16 +602,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="E5" s="2">
         <v>10</v>

</xml_diff>

<commit_message>
Worked on App config Static paths removed Sheet optimized Config updates Base inset script structure creation
</commit_message>
<xml_diff>
--- a/DbScript/Config.xlsx
+++ b/DbScript/Config.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Piyali\Tasks\Short_Term_Goal\TestdataGenerationTool\TestDataGen\DbScript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydutt\source\test\TestDataGen\DbScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669DF161-BCF7-416B-BB5C-0258178C32FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3874BF33-30E3-446A-ADE6-FDF92A399366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Common" sheetId="5" r:id="rId1"/>
-    <sheet name="Rules" sheetId="1" r:id="rId2"/>
+    <sheet name="Runner" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>OperationType</t>
   </si>
@@ -52,33 +51,9 @@
     <t>PersonNameActual</t>
   </si>
   <si>
-    <t>Database Connection</t>
-  </si>
-  <si>
-    <t>Database Name</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
-    <t>devsqlag.extendhealth.com</t>
-  </si>
-  <si>
-    <t>devehgalaxy</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Windows</t>
-  </si>
-  <si>
-    <t>Auth Type</t>
-  </si>
-  <si>
     <t>Update</t>
   </si>
   <si>
@@ -92,15 +67,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>DbServer</t>
-  </si>
-  <si>
-    <t>MSSQLSERVER</t>
-  </si>
-  <si>
-    <t>extendhealth\piroy</t>
   </si>
 </sst>
 </file>
@@ -170,13 +136,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,72 +419,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB6858C-092D-4812-BD96-35B3F9C96AE4}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
-    <col min="6" max="6" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,87 +435,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>11</v>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Insert script format- implemented few suggestions
</commit_message>
<xml_diff>
--- a/DbScript/Config.xlsx
+++ b/DbScript/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydutt\source\test\TestDataGen\DbScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3874BF33-30E3-446A-ADE6-FDF92A399366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E912F7-8CC2-4AA8-B18F-CCEF6DB46EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>OperationType</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -136,10 +139,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,99 +427,100 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="34.5546875" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="34.5546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1">
-        <v>10</v>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commits are related to Generate Random data & to check insertion_v1
</commit_message>
<xml_diff>
--- a/DbScript/Config.xlsx
+++ b/DbScript/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydutt\source\test\TestDataGen\DbScript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Piyali\Tasks\Short_Term_Goal\TestdataGenerationTool\TestDataGen\DbScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E912F7-8CC2-4AA8-B18F-CCEF6DB46EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188A20F4-197F-40C0-B974-BF6FDA21E7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>OperationType</t>
   </si>
   <si>
-    <t>Insert</t>
-  </si>
-  <si>
     <t>Required</t>
   </si>
   <si>
@@ -54,12 +51,6 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Update</t>
-  </si>
-  <si>
-    <t>Delete</t>
-  </si>
-  <si>
     <t>dbo</t>
   </si>
   <si>
@@ -70,6 +61,15 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>INSERT</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>DELETE</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,50 +441,50 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="E3" s="2">
         <v>10</v>
@@ -492,16 +492,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="E4" s="2">
         <v>10</v>
@@ -509,16 +509,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
         <v>10</v>
@@ -526,6 +526,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A5" xr:uid="{6C297F56-04D9-430B-A251-DB9FB38B627E}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5" xr:uid="{2D781564-B13C-453F-B4A6-ECABC7EF6715}">
+      <formula1>"INSERT,UPDATE,DELETE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commits are related to insert randomly generated data into DB_v1
</commit_message>
<xml_diff>
--- a/DbScript/Config.xlsx
+++ b/DbScript/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Piyali\Tasks\Short_Term_Goal\TestdataGenerationTool\TestDataGen\DbScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188A20F4-197F-40C0-B974-BF6FDA21E7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B640562-E98A-4B91-83A7-1330A0D0D907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,16 +60,16 @@
     <t>No</t>
   </si>
   <si>
+    <t>INSERT</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
     <t>10</t>
-  </si>
-  <si>
-    <t>INSERT</t>
-  </si>
-  <si>
-    <t>UPDATE</t>
-  </si>
-  <si>
-    <t>DELETE</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -470,7 +470,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -478,7 +478,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -495,7 +495,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -512,7 +512,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>

</xml_diff>